<commit_message>
updates in SRS, RTM, review document and CIL
</commit_message>
<xml_diff>
--- a/PM/CIL.xlsx
+++ b/PM/CIL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Internet Banking System Main\PM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36385AC2-1EAC-4FBF-B66B-C0B80F9EF9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3FEED9-C291-4678-BAE2-93C80CB5513A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>Configuration Items List</t>
   </si>
@@ -146,6 +146,18 @@
   </si>
   <si>
     <t>https://github.com/EsraaEMostafa/Internet-banking-system/blob/main/Code/internetbankingsystem.sql</t>
+  </si>
+  <si>
+    <t>V4.0</t>
+  </si>
+  <si>
+    <t>Review_Doc_1</t>
+  </si>
+  <si>
+    <t>Work product Review Comments</t>
+  </si>
+  <si>
+    <t>https://github.com/EsraaEMostafa/Internet-banking-system/blob/main/Requirements/Work%20product%20Review%20Comments.xlsx</t>
   </si>
 </sst>
 </file>
@@ -647,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,7 +771,7 @@
         <v>19</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>28</v>
@@ -821,11 +833,19 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
+    <row r="13" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
@@ -1074,6 +1094,7 @@
     <hyperlink ref="D10" r:id="rId8" xr:uid="{632424B7-A793-41EE-9102-E352A31866F0}"/>
     <hyperlink ref="D11" r:id="rId9" xr:uid="{B323B235-B3F2-44AD-9439-85EDF64C1F39}"/>
     <hyperlink ref="D12" r:id="rId10" xr:uid="{93185468-2C51-4274-B971-69DCED20AD33}"/>
+    <hyperlink ref="D13" r:id="rId11" xr:uid="{EB8C34C8-CA79-49B1-A243-1D4EC55992EE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>